<commit_message>
Modified to reflect changes to buffer for FLP request. Also, made a new function for Qinglin to convert linear_features to gr_skey pixel percent.
</commit_message>
<xml_diff>
--- a/data/analysis/stream_order_proxies_TSA.xlsx
+++ b/data/analysis/stream_order_proxies_TSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\THLB_Proxy\data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C2F66-053A-49EC-9968-999245A4DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63EB577-6FE2-429E-870E-2788612A1AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="300" windowWidth="26940" windowHeight="19320" activeTab="1" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
+    <workbookView xWindow="2660" yWindow="50" windowWidth="13100" windowHeight="10790" activeTab="1" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="152">
   <si>
     <t>Pacific</t>
   </si>
@@ -493,13 +493,19 @@
   </si>
   <si>
     <t>At this time there is not a data base that identifies a stream class for each stream reach within the Okanagan TSA. Instead of a specific riparian buffer for each stream class, a weighted average riparian buffer width across all streams, that was calculated for the Okanagan TSA based on an assessment of stream class distribution by Wild Stone Resources, will be used. This average reserve width of 12.4 metres is applied to each side of all streams (S1 to S6) identified in the Okanagan TSA timber supply review file (FWA-based streams).</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>FLP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,8 +528,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,6 +554,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -545,11 +571,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,12 +598,17 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1444,15 +1477,15 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20:T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="5" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="7.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.21875" style="8" bestFit="1" customWidth="1"/>
@@ -1643,37 +1676,37 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:23" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="11">
         <v>23</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="V4" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="13" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2350,68 +2383,68 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:23" s="11" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="11">
         <v>11</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="P20" s="11" t="s">
+      <c r="P20" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="Q20" s="11" t="s">
+      <c r="Q20" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="R20" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="T20" s="11" t="s">
+      <c r="R20" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="T20" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="U20" s="11" t="s">
+      <c r="U20" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="V20" s="9" t="s">
+      <c r="V20" s="11" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2776,68 +2809,68 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="9" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:23" s="11" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="11">
         <v>22</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="12">
         <v>12.4</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="12">
         <v>12.4</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="12">
         <v>12.4</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="12">
         <v>12.4</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="12">
         <v>12.4</v>
       </c>
-      <c r="I30" s="11">
+      <c r="I30" s="12">
         <v>12.4</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="12">
         <v>12.4</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K30" s="12">
         <v>10</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="12">
         <v>10</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="12">
         <v>15</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="12">
         <v>7.5</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="12">
         <v>7.5</v>
       </c>
-      <c r="P30" s="11">
+      <c r="P30" s="12">
         <v>20</v>
       </c>
-      <c r="Q30" s="11">
+      <c r="Q30" s="12">
         <v>15</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="12">
         <v>7.5</v>
       </c>
-      <c r="S30" s="11">
+      <c r="S30" s="12">
         <v>7.5</v>
       </c>
-      <c r="T30" s="11">
+      <c r="T30" s="12">
         <v>20</v>
       </c>
-      <c r="V30" s="9" t="s">
+      <c r="V30" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="W30" s="10" t="s">
+      <c r="W30" s="13" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3238,6 +3271,62 @@
       </c>
       <c r="T39" s="8">
         <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="R40" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="S40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="T40" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>